<commit_message>
Empleados, Tripulacion y Pasajero
</commit_message>
<xml_diff>
--- a/Proyecto_final/Insumos/base_menus.xlsx
+++ b/Proyecto_final/Insumos/base_menus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ovejo\Documents\Universidad-Daniel\Udea\Logica_y_representacion1\Trabajo-Logica---Aerolinea\Proyecto_final\Insumos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/67d5a1dced8d44fe/Documentos/Dirtrab/Trabajo-Logica---Aerolinea/Proyecto_final/Insumos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308B1C46-15F8-4E88-BB4F-CAD8045DDC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{308B1C46-15F8-4E88-BB4F-CAD8045DDC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4239BFC-B327-4DDD-BB86-DB47B8438472}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avion" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
   <si>
     <t>num_opcion</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Eli</t>
   </si>
   <si>
-    <t>Empleado</t>
-  </si>
-  <si>
     <t>Reporte general del hangar</t>
   </si>
   <si>
@@ -117,6 +114,21 @@
   </si>
   <si>
     <t>Actualizar datos pasajero</t>
+  </si>
+  <si>
+    <t>Nuevo empleado</t>
+  </si>
+  <si>
+    <t>Actualizar informacion del empleado</t>
+  </si>
+  <si>
+    <t>Actualizar el estado del empleado</t>
+  </si>
+  <si>
+    <t>Verificar disponibilidad para el vuelo</t>
+  </si>
+  <si>
+    <t>Informacion del empleado</t>
   </si>
 </sst>
 </file>
@@ -212,6 +224,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,7 +551,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -583,7 +599,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -613,7 +629,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -621,7 +637,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -629,7 +645,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -637,7 +653,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -645,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -653,7 +669,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -676,7 +692,9 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -697,7 +715,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -705,7 +723,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -713,7 +731,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -721,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -729,7 +747,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -737,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -775,7 +793,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -783,7 +801,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -791,7 +809,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1122,7 +1140,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1145,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1153,7 +1171,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1161,7 +1179,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>